<commit_message>
Automation of adding language test cases
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Data.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264CDC85-DA5A-456F-93AD-49704C2FDC27}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF2436C-D09C-4FDD-8B71-FC1E13D6F508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>French</t>
   </si>
@@ -403,7 +403,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,12 +426,14 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
Automation for skill and certificate
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Data.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Data.xlsx
@@ -3,27 +3,47 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF2436C-D09C-4FDD-8B71-FC1E13D6F508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D077A4-BCBE-45E8-BFBC-1EB5E649CEC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Language" sheetId="1" r:id="rId1"/>
+    <sheet name="certificate" sheetId="2" r:id="rId2"/>
+    <sheet name="skill" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>certificate</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>Industry Connect</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
   <si>
     <t>French</t>
   </si>
   <si>
-    <t>language</t>
-  </si>
-  <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -400,46 +420,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5840712-DAB0-49FB-9F6C-4CF71A1DD6B1}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB442556-9093-4C26-8440-A48A220A7FE9}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>